<commit_message>
commiting 3 files into git local repository
</commit_message>
<xml_diff>
--- a/test2.xlsx
+++ b/test2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9932b6e2ce60dae6/Documents/siddhant jaiswal office/study/gitlocalrepository/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_F25DC773A252ABDACC104826D9DF6A065BDE58F3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AF4494BA-51E7-4C52-AD98-42ED012EF1B1}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="11_F25DC773A252ABDACC104826D9DF6A065BDE58F3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{06E79B9C-B74D-4EC9-96B0-2E30E43ED2AD}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
-    <t xml:space="preserve">test2 this is </t>
+    <t>test2 this is good</t>
   </si>
 </sst>
 </file>
@@ -80,6 +80,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -347,7 +351,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>

</xml_diff>